<commit_message>
add workbook buffer reader
</commit_message>
<xml_diff>
--- a/labs/test-onetwo/src/test/resources/card.xlsx
+++ b/labs/test-onetwo/src/test/resources/card.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>cardNo</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,22 @@
   </si>
   <si>
     <t>cardType.cardBean.cardNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-111111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-222222</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-33333</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-44444</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -397,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -500,12 +516,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>111111111</v>
+      </c>
+      <c r="D2">
+        <v>5000</v>
+      </c>
+      <c r="E2">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>222222</v>
+      </c>
+      <c r="D3">
+        <v>5000</v>
+      </c>
+      <c r="E3">
+        <v>6677</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3333333</v>
+      </c>
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4444444</v>
+      </c>
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>